<commit_message>
added new annotations & renamed processes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Documents\UiPath\NK-Daily-Timesheet-RPA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\RPA\Git NK Daily-Timesheet-RPA-Master\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -123,7 +123,10 @@
     <t>zoho_timesheet_orc</t>
   </si>
   <si>
-    <t>AIpass123456</t>
+    <t>Zoho_Timesheet_Asset
+Zoho_Timesheet_Asset
+Zoho_Timesheet_Asset
+Zoho_Timesheet_Asset</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -574,7 +577,7 @@
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
another round of changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\RPA\Git NK Daily-Timesheet-RPA-Master\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Documents\UiPath\Git NK Daily-Timesheet-RPA-Master\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -86,13 +86,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -123,17 +116,32 @@
     <t>zoho_timesheet_orc</t>
   </si>
   <si>
-    <t>Zoho_Timesheet_Asset
-Zoho_Timesheet_Asset
-Zoho_Timesheet_Asset
-Zoho_Timesheet_Asset</t>
+    <t>ZohoProcess</t>
+  </si>
+  <si>
+    <t>Zoho_Timesheet_Asset</t>
+  </si>
+  <si>
+    <t>Zoho_Queue</t>
+  </si>
+  <si>
+    <t>ZohoURL</t>
+  </si>
+  <si>
+    <t>https://accounts.zoho.com/signin</t>
+  </si>
+  <si>
+    <t>Orchestrator asset Name. The value must match with the asset name defined on Orchestrator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoho book sign in link </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,6 +165,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -175,10 +189,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -188,8 +203,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,7 +525,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -552,13 +572,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -566,22 +586,35 @@
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1575,8 +1608,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1636,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1660,7 +1696,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1682,7 +1718,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1693,7 +1729,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1704,7 +1740,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>